<commit_message>
got list of classes to work on excel
</commit_message>
<xml_diff>
--- a/testingSheetJS.xlsx
+++ b/testingSheetJS.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20228"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58FF46FC-E1F5-41D6-B7B3-743127E38417}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01716F92-8EC1-409A-9E2C-AD3C502650B4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12960" windowHeight="8544" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>Names</t>
   </si>
@@ -79,12 +79,6 @@
   </si>
   <si>
     <t>Date</t>
-  </si>
-  <si>
-    <t>A+</t>
-  </si>
-  <si>
-    <t>A-</t>
   </si>
   <si>
     <t>Period</t>
@@ -244,6 +238,30 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{DFA65E25-875A-46DF-871D-B33B1C73114B}" name="Table1" displayName="Table1" ref="A1:L6" totalsRowShown="0">
+  <autoFilter ref="A1:L6" xr:uid="{03B65F66-594A-4BF9-9FE0-833B0DA04EC1}"/>
+  <sortState ref="A2:L6">
+    <sortCondition ref="A1:A6"/>
+  </sortState>
+  <tableColumns count="12">
+    <tableColumn id="1" xr3:uid="{729EEA5F-B2DE-4EE0-A8E7-63C2AD0A38D0}" name="ID's"/>
+    <tableColumn id="2" xr3:uid="{DC10CC59-5E58-49DA-949E-ED8A6CDFDEC4}" name="Names"/>
+    <tableColumn id="3" xr3:uid="{0263ACD4-936F-434F-BD93-D26E9CD94CFB}" name="Unimportant"/>
+    <tableColumn id="4" xr3:uid="{945D7550-EA0D-4421-9789-AF271EB4E344}" name="Dumb"/>
+    <tableColumn id="5" xr3:uid="{FD9BF339-11A8-49DF-B5AA-BB4E26C35194}" name="Class 1"/>
+    <tableColumn id="6" xr3:uid="{352A60B6-D301-4C95-A152-39C3B1A14181}" name="Class 2"/>
+    <tableColumn id="7" xr3:uid="{611C2254-212F-4989-AB73-F341D9C8E51A}" name="Class 3"/>
+    <tableColumn id="8" xr3:uid="{2C96255B-8A74-4C00-A8FF-407358A5F78F}" name="Class 4"/>
+    <tableColumn id="9" xr3:uid="{4C2F64B9-6085-43A7-9EFF-24B2587AADE2}" name="Class 5"/>
+    <tableColumn id="10" xr3:uid="{A902FDC5-C79E-4116-8ABE-6089FFE52EB7}" name="Class 6"/>
+    <tableColumn id="11" xr3:uid="{E9CDE10B-F14A-4FB3-B9B2-1D60F27991D8}" name="Class 7"/>
+    <tableColumn id="12" xr3:uid="{6AF8D16A-1D2E-4EB5-BE0A-CED19538CA51}" name="Class 8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -509,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -524,7 +542,7 @@
     <col min="11" max="11" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -550,94 +568,82 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="str">
         <f>IF(A2 &lt;&gt; "",VLOOKUP($A2,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
-        <v>Larry</v>
+        <v>Joan</v>
       </c>
       <c r="C2">
         <f>IF(A2 &lt;&gt; "", VLOOKUP($A2,'Student reference sheet'!$A$2:$D$12, 3,FALSE), "")</f>
-        <v>423432</v>
+        <v>234234</v>
       </c>
       <c r="D2" t="str">
         <f>IF(A2 &lt;&gt; "", VLOOKUP($A2,'Student reference sheet'!$A$2:$D$12, 4,FALSE), "")</f>
-        <v>dog</v>
+        <v>name</v>
       </c>
       <c r="E2">
         <f>IF(A2 &lt;&gt; "", 1, "")</f>
         <v>1</v>
       </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
       <c r="G2" s="3">
         <f ca="1">IF(A2 &lt;&gt;"", IF(G2 = "",NOW() - TODAY(), G2), "")</f>
-        <v>0.42799155092507135</v>
+        <v>0.5820304398148437</v>
       </c>
       <c r="H2" s="4">
         <f ca="1">IF(A2 &lt;&gt;"", IF(H2 = "",TODAY(), H2), "")</f>
-        <v>43307</v>
+        <v>43309</v>
       </c>
       <c r="I2" s="5">
         <f ca="1">IF(A2 &lt;&gt; "",VLOOKUP(G2,'Bell Schedule Reference'!$A$3:$B$11,2,TRUE), "")</f>
-        <v>3</v>
-      </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5">
-        <f ca="1">G2</f>
-        <v>0.42799155092507135</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
         <f>IF(A3 &lt;&gt; "",VLOOKUP($A3,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
-        <v>Jim</v>
+        <v>Larry</v>
       </c>
       <c r="C3">
         <f>IF(A3 &lt;&gt; "", VLOOKUP($A3,'Student reference sheet'!$A$2:$D$12, 3,FALSE), "")</f>
-        <v>56667</v>
+        <v>423432</v>
       </c>
       <c r="D3" t="str">
         <f>IF(A3 &lt;&gt; "", VLOOKUP($A3,'Student reference sheet'!$A$2:$D$12, 4,FALSE), "")</f>
-        <v>my</v>
+        <v>dog</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E12" si="0">IF(A3 &lt;&gt; "", 1, "")</f>
+        <f t="shared" ref="E3:E8" si="0">IF(A3 &lt;&gt; "", 1, "")</f>
         <v>1</v>
       </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
       <c r="G3" s="3">
-        <f t="shared" ref="G3:G12" ca="1" si="1">IF(A3 &lt;&gt;"", IF(G3 = "",NOW() - TODAY(), G3), "")</f>
-        <v>0.42826921296364162</v>
+        <f t="shared" ref="G3:G8" ca="1" si="1">IF(A3 &lt;&gt;"", IF(G3 = "",NOW() - TODAY(), G3), "")</f>
+        <v>0.58241018518310739</v>
       </c>
       <c r="H3" s="4">
-        <f t="shared" ref="H3:H12" ca="1" si="2">IF(A3 &lt;&gt;"", IF(H3 = "",TODAY(), H3), "")</f>
-        <v>43307</v>
+        <f t="shared" ref="H3:H8" ca="1" si="2">IF(A3 &lt;&gt;"", IF(H3 = "",TODAY(), H3), "")</f>
+        <v>43309</v>
       </c>
       <c r="I3" s="5">
         <f ca="1">IF(A3 &lt;&gt; "",VLOOKUP(G3,'Bell Schedule Reference'!$A$3:$B$11,2,TRUE), "")</f>
-        <v>3</v>
-      </c>
-      <c r="K3">
-        <v>91</v>
-      </c>
-      <c r="L3" t="str">
-        <f>VLOOKUP(K3,N3:O7,2,TRUE)</f>
-        <v>A-</v>
-      </c>
-      <c r="N3">
-        <v>90</v>
-      </c>
-      <c r="O3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B4" t="str">
         <f>IF(A4 &lt;&gt; "",VLOOKUP($A4,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -666,14 +672,8 @@
         <f>IF(A4 &lt;&gt; "",VLOOKUP(G4,'Bell Schedule Reference'!$A$3:$B$11,2,TRUE), "")</f>
         <v/>
       </c>
-      <c r="N4">
-        <v>100</v>
-      </c>
-      <c r="O4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5" t="str">
         <f>IF(A5 &lt;&gt; "",VLOOKUP($A5,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -703,7 +703,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B6" t="str">
         <f>IF(A6 &lt;&gt; "",VLOOKUP($A6,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -733,7 +733,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" t="str">
         <f>IF(A7 &lt;&gt; "",VLOOKUP($A7,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -763,7 +763,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B8" t="str">
         <f>IF(A8 &lt;&gt; "",VLOOKUP($A8,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -793,7 +793,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B9" t="str">
         <f>IF(A9 &lt;&gt; "",VLOOKUP($A9,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -802,28 +802,8 @@
         <f>IF(A9 &lt;&gt; "", VLOOKUP($A9,'Student reference sheet'!$A$2:$D$12, 3,FALSE), "")</f>
         <v/>
       </c>
-      <c r="D9" t="str">
-        <f>IF(A9 &lt;&gt; "", VLOOKUP($A9,'Student reference sheet'!$A$2:$D$12, 4,FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="E9" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G9" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="H9" s="4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="I9" s="5" t="str">
-        <f>IF(A9 &lt;&gt; "",VLOOKUP(G9,'Bell Schedule Reference'!$A$3:$B$11,2,TRUE), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" t="str">
         <f>IF(A10 &lt;&gt; "",VLOOKUP($A10,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -832,28 +812,8 @@
         <f>IF(A10 &lt;&gt; "", VLOOKUP($A10,'Student reference sheet'!$A$2:$D$12, 3,FALSE), "")</f>
         <v/>
       </c>
-      <c r="D10" t="str">
-        <f>IF(A10 &lt;&gt; "", VLOOKUP($A10,'Student reference sheet'!$A$2:$D$12, 4,FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="E10" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G10" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="H10" s="4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="I10" s="5" t="str">
-        <f>IF(A10 &lt;&gt; "",VLOOKUP(G10,'Bell Schedule Reference'!$A$3:$B$11,2,TRUE), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" t="str">
         <f>IF(A11 &lt;&gt; "",VLOOKUP($A11,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -862,28 +822,8 @@
         <f>IF(A11 &lt;&gt; "", VLOOKUP($A11,'Student reference sheet'!$A$2:$D$12, 3,FALSE), "")</f>
         <v/>
       </c>
-      <c r="D11" t="str">
-        <f>IF(A11 &lt;&gt; "", VLOOKUP($A11,'Student reference sheet'!$A$2:$D$12, 4,FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="E11" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G11" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="H11" s="4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="I11" s="5" t="str">
-        <f>IF(A11 &lt;&gt; "",VLOOKUP(G11,'Bell Schedule Reference'!$A$3:$B$11,2,TRUE), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" t="str">
         <f>IF(A12 &lt;&gt; "",VLOOKUP($A12,'Student reference sheet'!$A$2:$D$12, 2,FALSE), "")</f>
         <v/>
@@ -892,46 +832,18 @@
         <f>IF(A12 &lt;&gt; "", VLOOKUP($A12,'Student reference sheet'!$A$2:$D$12, 3,FALSE), "")</f>
         <v/>
       </c>
-      <c r="D12" t="str">
-        <f>IF(A12 &lt;&gt; "", VLOOKUP($A12,'Student reference sheet'!$A$2:$D$12, 4,FALSE), "")</f>
-        <v/>
-      </c>
-      <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="G12" s="3" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v/>
-      </c>
-      <c r="H12" s="4" t="str">
-        <f t="shared" ca="1" si="2"/>
-        <v/>
-      </c>
-      <c r="I12" s="5" t="str">
-        <f>IF(A12 &lt;&gt; "",VLOOKUP(G12,'Bell Schedule Reference'!$A$3:$B$11,2,TRUE), "")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="G16" s="3"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2" xr:uid="{941FC29D-1A4D-47CF-B069-5766D54667C5}">
-      <formula1>IF(A2&lt;&gt;"", A3, A4)</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{06ED612F-A69F-4BF6-9E45-D1A221083377}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{941FC29D-1A4D-47CF-B069-5766D54667C5}">
           <x14:formula1>
-            <xm:f>'Student reference sheet'!$E$2:$L$2</xm:f>
+            <xm:f>OFFSET('Student reference sheet'!$A$2,MATCH($A2,'Student reference sheet'!$A$2:$A$6) - 1,4,1,7)</xm:f>
           </x14:formula1>
-          <xm:sqref>F3:F10</xm:sqref>
+          <xm:sqref>F2:F8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -944,10 +856,13 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -963,98 +878,98 @@
         <v>8</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
-      </c>
-      <c r="K1" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2">
-        <v>423432</v>
+        <v>2233</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>42</v>
+      </c>
+      <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" t="s">
-        <v>36</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-      <c r="J2" t="s">
-        <v>46</v>
-      </c>
-      <c r="K2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
-        <v>2233</v>
+        <v>423432</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="G3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" t="s">
+        <v>35</v>
+      </c>
+      <c r="J3" t="s">
         <v>44</v>
       </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
       <c r="K3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -1071,25 +986,25 @@
         <v>11</v>
       </c>
       <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G4" t="s">
         <v>44</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H4" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" t="s">
         <v>36</v>
-      </c>
-      <c r="G4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1106,25 +1021,25 @@
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I5" t="s">
         <v>35</v>
       </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" t="s">
-        <v>37</v>
-      </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -1141,29 +1056,32 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="K6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -1172,7 +1090,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1183,7 +1101,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="6"/>
     </row>
@@ -1192,7 +1110,7 @@
         <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1260,7 +1178,7 @@
         <v>0.52430555555555558</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
@@ -1296,7 +1214,7 @@
         <v>0.62638888888888888</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="5">
         <f t="shared" si="0"/>

</xml_diff>